<commit_message>
Update Kho gửi phòng SX-BH 01_2026.xlsx
</commit_message>
<xml_diff>
--- a/5. Other/Thiết bị kho gửi/2026/Kho gửi phòng SX-BH 01_2026.xlsx
+++ b/5. Other/Thiết bị kho gửi/2026/Kho gửi phòng SX-BH 01_2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNET\5. Other\Thiết bị kho gửi\2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A109A2A-FF86-4524-81CB-1AA6886652D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044FDB59-F4C1-41AE-A685-2B6AA90BFF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhập xuất tồn" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="56">
   <si>
     <t>VNSH01</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Đã trả (13/01/26)</t>
+  </si>
+  <si>
+    <t>ĐL Anh Thái QN</t>
+  </si>
+  <si>
+    <t>Chưa trả</t>
+  </si>
+  <si>
+    <t>ĐL Anh Sửu Bình Định</t>
   </si>
 </sst>
 </file>
@@ -355,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,14 +459,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4547,10 +4553,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C51F44-131D-46D9-8F20-A11BD47AE60F}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4635,7 +4641,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="A6" s="30">
         <v>45663</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -4650,7 +4656,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
@@ -4736,7 +4742,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
+      <c r="A13" s="30">
         <v>45670</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -4751,7 +4757,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
@@ -4764,26 +4770,132 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="33">
+        <v>45671</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="D15" s="9">
+        <v>10</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="D16" s="9">
+        <v>10</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E7" xr:uid="{171653DB-B967-4059-9CE3-FD13B7B63DBC}"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:E1000">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -4801,7 +4913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1D2FD3-91FF-42CA-8178-C2AD22F246DD}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showZeros="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -5282,10 +5394,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="18">
         <f>SUM(C3:C17)</f>
         <v>157</v>

</xml_diff>